<commit_message>
Added test data iterator
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FA1AF7E4-8419-40C6-AC9F-F8FF06814156}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0F601C5B-0157-4AA3-BA38-C17D9E7C46F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BasicSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -437,7 +437,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added subsite URL and test; cleaned up data providers
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AA7710E-7DD0-4BC1-BFDE-660D2DE1A28E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2D77DE8-5A36-4F6D-9F96-5133FCC1B7D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
+    <sheet name="SitewideSearchEs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>breast</t>
   </si>
@@ -94,6 +95,42 @@
   </si>
   <si>
     <t>LiveHelp</t>
+  </si>
+  <si>
+    <t>dolor</t>
+  </si>
+  <si>
+    <t>tabaco</t>
+  </si>
+  <si>
+    <t>linfoma</t>
+  </si>
+  <si>
+    <t>cáncer</t>
+  </si>
+  <si>
+    <t>cáncer de hígado</t>
+  </si>
+  <si>
+    <t>A33</t>
+  </si>
+  <si>
+    <t>safingol</t>
+  </si>
+  <si>
+    <t>dalteparina sódica</t>
+  </si>
+  <si>
+    <t>macrófago</t>
+  </si>
+  <si>
+    <t>dermis</t>
+  </si>
+  <si>
+    <t>TAC-101</t>
+  </si>
+  <si>
+    <t>lanolina</t>
   </si>
 </sst>
 </file>
@@ -464,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,4 +607,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged "bacon" dev branch into "sitewide-search" feature branch (#70)
* Added getBeacons() methods
* Added local "beacon" variable to each test class
* Moved has...() methods from AnalyticsTestBase to AnalyticsRequest
* Updated method call in test asserts
* Removed set() beacon methods
* Moved MegaMenu into commonobjects package
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2D77DE8-5A36-4F6D-9F96-5133FCC1B7D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1FD299CB-95F4-4F26-B753-AA9819525A16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SitewideSearch" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>argle-bargle</t>
   </si>
   <si>
-    <t xml:space="preserve"> Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
-  </si>
-  <si>
     <t>CancerTerm</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>lanolina</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,19 +516,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -553,49 +553,49 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6634F395-7540-4542-954F-5DFBBE6DB702}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -626,66 +626,66 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored shared assertions in SitewideSearch_Test
</commit_message>
<xml_diff>
--- a/test-data/sitewide-search.xlsx
+++ b/test-data/sitewide-search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1FD299CB-95F4-4F26-B753-AA9819525A16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F5C256A7-ABF6-4BE8-BE96-888FABB7C166}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>shark</t>
   </si>
   <si>
-    <t>argle-bargle</t>
-  </si>
-  <si>
     <t>CancerTerm</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Cras vitae neque consectetur, fringilla nunc eget, faucibus sem. Nulla aliquet imperdiet arcu, non dapibus lorem tincidunt pharetra. Donec sollicitudin risus sit amet eros facilisis eleifend. Donec</t>
+  </si>
+  <si>
+    <t>argle-bargle or foofaraw</t>
   </si>
 </sst>
 </file>
@@ -501,9 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -516,19 +514,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -536,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -545,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -553,49 +551,49 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,66 +624,66 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>